<commit_message>
Latest changes - sorry
</commit_message>
<xml_diff>
--- a/test_data/Batch.xlsx
+++ b/test_data/Batch.xlsx
@@ -24,79 +24,79 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="25">
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Take Off</t>
-  </si>
-  <si>
-    <t>Amplification</t>
-  </si>
-  <si>
-    <t>Comparative Conc.</t>
-  </si>
-  <si>
-    <t>Rep. Takeoff</t>
-  </si>
-  <si>
-    <t>Rep. Takeoff (95% CI)</t>
-  </si>
-  <si>
-    <t>Rep. Amp.</t>
-  </si>
-  <si>
-    <t>Rep. Amp. (95% CI)</t>
-  </si>
-  <si>
-    <t>Rep. Conc.</t>
-  </si>
-  <si>
-    <t>Rep. Calibrator</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>t</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>ts</t>
-  </si>
-  <si>
-    <t>ave ts</t>
-  </si>
-  <si>
-    <t>cv</t>
-  </si>
-  <si>
-    <t>error code</t>
-  </si>
-  <si>
-    <t>pool</t>
-  </si>
-  <si>
-    <t>[13.0 , 13.2]</t>
-  </si>
-  <si>
-    <t>[1.74 , 1.78]</t>
-  </si>
-  <si>
-    <t>Calibrator</t>
-  </si>
-  <si>
-    <t>[20.9 , 21.1]</t>
-  </si>
-  <si>
-    <t>[1.73 , 1.76]</t>
-  </si>
-  <si>
-    <t>mean</t>
-  </si>
-  <si>
-    <t>median</t>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take Off</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amplification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comparative Conc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rep. Takeoff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rep. Takeoff (95% CI)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rep. Amp.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rep. Amp. (95% CI)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rep. Conc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rep. Calibrator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ave ts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">error code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[13.0 , 13.2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1.74 , 1.78]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calibrator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[20.9 , 21.1]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1.73 , 1.76]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">median</t>
   </si>
 </sst>
 </file>
@@ -104,7 +104,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
     <numFmt numFmtId="166" formatCode="0.00E+00"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
@@ -248,8 +248,8 @@
   </sheetPr>
   <dimension ref="A1:AD33"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AD1" activeCellId="0" sqref="1:1048576"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AC2" activeCellId="0" sqref="AC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -403,7 +403,7 @@
       <c r="AB2" s="0"/>
       <c r="AC2" s="0"/>
       <c r="AD2" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -455,7 +455,7 @@
         <v>0.362768890637698</v>
       </c>
       <c r="AD3" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1791,7 +1791,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1817,7 +1817,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Ignore samples with and 8 or 9
</commit_message>
<xml_diff>
--- a/test_data/Batch.xlsx
+++ b/test_data/Batch.xlsx
@@ -249,7 +249,7 @@
   <dimension ref="A1:AD33"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AC2" activeCellId="0" sqref="AC2"/>
+      <selection pane="topLeft" activeCell="AD21" activeCellId="0" sqref="AD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1325,7 +1325,7 @@
       <c r="AB18" s="0"/>
       <c r="AC18" s="0"/>
       <c r="AD18" s="0" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1441,7 +1441,7 @@
       <c r="AB20" s="0"/>
       <c r="AC20" s="0"/>
       <c r="AD20" s="0" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>